<commit_message>
Improve numerical stability on input data
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/FragilityCurvesData/PercentageHurricaneDamage.xlsx
+++ b/CreateBaseDeck/FragilityCurvesData/PercentageHurricaneDamage.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L140"/>
+  <dimension ref="A1:K140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,11 +489,6 @@
           <t>S1</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -519,22 +514,19 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.004971784630030634</v>
+        <v>0.005</v>
       </c>
       <c r="H2" t="n">
-        <v>0.05009376689305815</v>
+        <v>0.0501</v>
       </c>
       <c r="I2" t="n">
-        <v>0.09744070550223795</v>
+        <v>0.0974</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.02781089530481343</v>
+        <v>0.0124</v>
       </c>
     </row>
     <row r="3">
@@ -549,34 +541,31 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.006574540822656515</v>
+        <v>0.0066</v>
       </c>
       <c r="D3" t="n">
-        <v>0.006100325238603099</v>
+        <v>0.0061</v>
       </c>
       <c r="E3" t="n">
-        <v>0.005771691266480976</v>
+        <v>0.0058</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0126371904711061</v>
+        <v>0.0126</v>
       </c>
       <c r="G3" t="n">
-        <v>0.04114308769540496</v>
+        <v>0.0411</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1164393967949617</v>
+        <v>0.1164</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1961850683753682</v>
+        <v>0.1962</v>
       </c>
       <c r="J3" t="n">
-        <v>0.001000488923280464</v>
+        <v>0.0011</v>
       </c>
       <c r="K3" t="n">
-        <v>0.008060191001356017</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.07934741255528956</v>
+        <v>0.0423</v>
       </c>
     </row>
     <row r="4">
@@ -591,34 +580,31 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.006574540822656515</v>
+        <v>0.0066</v>
       </c>
       <c r="D4" t="n">
-        <v>0.006100325238603099</v>
+        <v>0.0061</v>
       </c>
       <c r="E4" t="n">
-        <v>0.005771691266480976</v>
+        <v>0.0058</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0126371904711061</v>
+        <v>0.0126</v>
       </c>
       <c r="G4" t="n">
-        <v>0.04114308769540496</v>
+        <v>0.0411</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1164393967949617</v>
+        <v>0.1164</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1961850683753682</v>
+        <v>0.1962</v>
       </c>
       <c r="J4" t="n">
-        <v>0.001000488923280464</v>
+        <v>0.0011</v>
       </c>
       <c r="K4" t="n">
-        <v>0.008060191001356017</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.07934741255528956</v>
+        <v>0.0423</v>
       </c>
     </row>
     <row r="5">
@@ -633,34 +619,31 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.006574540822656515</v>
+        <v>0.0066</v>
       </c>
       <c r="D5" t="n">
-        <v>0.006100325238603099</v>
+        <v>0.0061</v>
       </c>
       <c r="E5" t="n">
-        <v>0.005771691266480976</v>
+        <v>0.0058</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0126371904711061</v>
+        <v>0.0126</v>
       </c>
       <c r="G5" t="n">
-        <v>0.04114308769540496</v>
+        <v>0.0411</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1164393967949617</v>
+        <v>0.1164</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1961850683753682</v>
+        <v>0.1962</v>
       </c>
       <c r="J5" t="n">
-        <v>0.001000488923280464</v>
+        <v>0.0011</v>
       </c>
       <c r="K5" t="n">
-        <v>0.008060191001356017</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.07934741255528956</v>
+        <v>0.0423</v>
       </c>
     </row>
     <row r="6">
@@ -675,34 +658,31 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.006574540822656515</v>
+        <v>0.0066</v>
       </c>
       <c r="D6" t="n">
-        <v>0.006100325238603099</v>
+        <v>0.0061</v>
       </c>
       <c r="E6" t="n">
-        <v>0.005771691266480976</v>
+        <v>0.0058</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0126371904711061</v>
+        <v>0.0126</v>
       </c>
       <c r="G6" t="n">
-        <v>0.04114308769540496</v>
+        <v>0.0411</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1164393967949617</v>
+        <v>0.1164</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1961850683753682</v>
+        <v>0.1962</v>
       </c>
       <c r="J6" t="n">
-        <v>0.001000488923280464</v>
+        <v>0.0011</v>
       </c>
       <c r="K6" t="n">
-        <v>0.008060191001356017</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.07934741255528956</v>
+        <v>0.0423</v>
       </c>
     </row>
     <row r="7">
@@ -726,25 +706,22 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.000437837822876621</v>
+        <v>0.0004</v>
       </c>
       <c r="G7" t="n">
-        <v>0.01026032967390825</v>
+        <v>0.0103</v>
       </c>
       <c r="H7" t="n">
-        <v>0.06332597753187813</v>
+        <v>0.0633</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1399637247335608</v>
+        <v>0.14</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0001459459409588737</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.03973966602085729</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="8">
@@ -768,25 +745,22 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.000437837822876621</v>
+        <v>0.0004</v>
       </c>
       <c r="G8" t="n">
-        <v>0.01026032967390825</v>
+        <v>0.0103</v>
       </c>
       <c r="H8" t="n">
-        <v>0.06332597753187813</v>
+        <v>0.0633</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1399637247335608</v>
+        <v>0.14</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0001459459409588737</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.03973966602085729</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="9">
@@ -804,31 +778,28 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>2.491562421045714e-05</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.01647931439678806</v>
+        <v>0.0165</v>
       </c>
       <c r="F9" t="n">
-        <v>0.03398437233585025</v>
+        <v>0.034</v>
       </c>
       <c r="G9" t="n">
-        <v>0.05582176575723141</v>
+        <v>0.0558</v>
       </c>
       <c r="H9" t="n">
-        <v>0.09846365966035799</v>
+        <v>0.0985</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1360753301288614</v>
+        <v>0.1361</v>
       </c>
       <c r="J9" t="n">
-        <v>1.294990863329373e-06</v>
+        <v>0.0003</v>
       </c>
       <c r="K9" t="n">
-        <v>0.02231433370980879</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.0765139347794668</v>
+        <v>0.0529</v>
       </c>
     </row>
     <row r="10">
@@ -852,25 +823,22 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.000437837822876621</v>
+        <v>0.0004</v>
       </c>
       <c r="G10" t="n">
-        <v>0.01026032967390825</v>
+        <v>0.0103</v>
       </c>
       <c r="H10" t="n">
-        <v>0.06332597753187813</v>
+        <v>0.0633</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1399637247335608</v>
+        <v>0.14</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0001459459409588737</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.03973966602085729</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="11">
@@ -894,25 +862,22 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.000437837822876621</v>
+        <v>0.0004</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01026032967390825</v>
+        <v>0.0103</v>
       </c>
       <c r="H11" t="n">
-        <v>0.06332597753187813</v>
+        <v>0.0633</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1399637247335608</v>
+        <v>0.14</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0001459459409588737</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.03973966602085729</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="12">
@@ -936,25 +901,22 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.000437837822876621</v>
+        <v>0.0004</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01026032967390825</v>
+        <v>0.0103</v>
       </c>
       <c r="H12" t="n">
-        <v>0.06332597753187813</v>
+        <v>0.0633</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1399637247335608</v>
+        <v>0.14</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0001459459409588737</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.03973966602085729</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="13">
@@ -978,25 +940,22 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0001681340776008133</v>
+        <v>0.0002</v>
       </c>
       <c r="G13" t="n">
-        <v>0.009277398210473457</v>
+        <v>0.009299999999999999</v>
       </c>
       <c r="H13" t="n">
-        <v>0.05674783467615626</v>
+        <v>0.0567</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1035408050587893</v>
+        <v>0.1035</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>5.604469253360444e-05</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.03292793318293364</v>
+        <v>0.0147</v>
       </c>
     </row>
     <row r="14">
@@ -1023,22 +982,19 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.005084644734054182</v>
+        <v>0.0051</v>
       </c>
       <c r="H14" t="n">
-        <v>0.03185879734240016</v>
+        <v>0.0319</v>
       </c>
       <c r="I14" t="n">
-        <v>0.06478170440187801</v>
+        <v>0.0648</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.01924031534461865</v>
+        <v>0.0086</v>
       </c>
     </row>
     <row r="15">
@@ -1056,31 +1012,28 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>2.491562421045714e-05</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.01647931439678806</v>
+        <v>0.0165</v>
       </c>
       <c r="F15" t="n">
-        <v>0.03398437233585025</v>
+        <v>0.034</v>
       </c>
       <c r="G15" t="n">
-        <v>0.05582176575723141</v>
+        <v>0.0558</v>
       </c>
       <c r="H15" t="n">
-        <v>0.09846365966035799</v>
+        <v>0.0985</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1360753301288614</v>
+        <v>0.1361</v>
       </c>
       <c r="J15" t="n">
-        <v>1.294990863329373e-06</v>
+        <v>0.0003</v>
       </c>
       <c r="K15" t="n">
-        <v>0.02231433370980879</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.0765139347794668</v>
+        <v>0.0529</v>
       </c>
     </row>
     <row r="16">
@@ -1121,9 +1074,6 @@
       <c r="K16" t="n">
         <v>0</v>
       </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1163,9 +1113,6 @@
       <c r="K17" t="n">
         <v>0</v>
       </c>
-      <c r="L17" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1205,9 +1152,6 @@
       <c r="K18" t="n">
         <v>0</v>
       </c>
-      <c r="L18" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1247,9 +1191,6 @@
       <c r="K19" t="n">
         <v>0</v>
       </c>
-      <c r="L19" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1289,9 +1230,6 @@
       <c r="K20" t="n">
         <v>0</v>
       </c>
-      <c r="L20" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1311,28 +1249,25 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.001856934960681747</v>
+        <v>0.0019</v>
       </c>
       <c r="F21" t="n">
-        <v>0.01740434783660504</v>
+        <v>0.0174</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0489356192275605</v>
+        <v>0.0489</v>
       </c>
       <c r="H21" t="n">
-        <v>0.1847037410119856</v>
+        <v>0.1847</v>
       </c>
       <c r="I21" t="n">
-        <v>0.3517995272232919</v>
+        <v>0.3518</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>0.007039405919322844</v>
-      </c>
-      <c r="L21" t="n">
-        <v>0.1207356381731332</v>
+        <v>0.0633</v>
       </c>
     </row>
     <row r="22">
@@ -1359,22 +1294,19 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>0.007542746542774958</v>
+        <v>0.0075</v>
       </c>
       <c r="H22" t="n">
-        <v>0.05710721674366193</v>
+        <v>0.0571</v>
       </c>
       <c r="I22" t="n">
-        <v>0.1383121899472384</v>
+        <v>0.1383</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0.03628004451855464</v>
+        <v>0.0161</v>
       </c>
     </row>
     <row r="23">
@@ -1398,25 +1330,22 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.000437837822876621</v>
+        <v>0.0004</v>
       </c>
       <c r="G23" t="n">
-        <v>0.01026032967390825</v>
+        <v>0.0103</v>
       </c>
       <c r="H23" t="n">
-        <v>0.06332597753187813</v>
+        <v>0.0633</v>
       </c>
       <c r="I23" t="n">
-        <v>0.1399637247335608</v>
+        <v>0.14</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0001459459409588737</v>
-      </c>
-      <c r="L23" t="n">
-        <v>0.03973966602085729</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="24">
@@ -1440,25 +1369,22 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.000437837822876621</v>
+        <v>0.0004</v>
       </c>
       <c r="G24" t="n">
-        <v>0.01026032967390825</v>
+        <v>0.0103</v>
       </c>
       <c r="H24" t="n">
-        <v>0.06332597753187813</v>
+        <v>0.0633</v>
       </c>
       <c r="I24" t="n">
-        <v>0.1399637247335608</v>
+        <v>0.14</v>
       </c>
       <c r="J24" t="n">
         <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0001459459409588737</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0.03973966602085729</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="25">
@@ -1482,25 +1408,22 @@
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0.000437837822876621</v>
+        <v>0.0004</v>
       </c>
       <c r="G25" t="n">
-        <v>0.01026032967390825</v>
+        <v>0.0103</v>
       </c>
       <c r="H25" t="n">
-        <v>0.06332597753187813</v>
+        <v>0.0633</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1399637247335608</v>
+        <v>0.14</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>0.0001459459409588737</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0.03973966602085729</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="26">
@@ -1524,25 +1447,22 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0.000437837822876621</v>
+        <v>0.0004</v>
       </c>
       <c r="G26" t="n">
-        <v>0.01026032967390825</v>
+        <v>0.0103</v>
       </c>
       <c r="H26" t="n">
-        <v>0.06332597753187813</v>
+        <v>0.0633</v>
       </c>
       <c r="I26" t="n">
-        <v>0.1399637247335608</v>
+        <v>0.14</v>
       </c>
       <c r="J26" t="n">
         <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>0.0001459459409588737</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0.03973966602085729</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="27">
@@ -1566,25 +1486,22 @@
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0008214154688869933</v>
+        <v>0.0008</v>
       </c>
       <c r="G27" t="n">
-        <v>0.01413955539436815</v>
+        <v>0.0141</v>
       </c>
       <c r="H27" t="n">
-        <v>0.07796909117120662</v>
+        <v>0.078</v>
       </c>
       <c r="I27" t="n">
-        <v>0.1751467313695733</v>
+        <v>0.1751</v>
       </c>
       <c r="J27" t="n">
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>0.0002738051562956645</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0.05022283633547842</v>
+        <v>0.0228</v>
       </c>
     </row>
     <row r="28">
@@ -1608,25 +1525,22 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.000437837822876621</v>
+        <v>0.0004</v>
       </c>
       <c r="G28" t="n">
-        <v>0.01026032967390825</v>
+        <v>0.0103</v>
       </c>
       <c r="H28" t="n">
-        <v>0.06332597753187813</v>
+        <v>0.0633</v>
       </c>
       <c r="I28" t="n">
-        <v>0.1399637247335608</v>
+        <v>0.14</v>
       </c>
       <c r="J28" t="n">
         <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>0.0001459459409588737</v>
-      </c>
-      <c r="L28" t="n">
-        <v>0.03973966602085729</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="29">
@@ -1650,25 +1564,22 @@
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0.000437837822876621</v>
+        <v>0.0004</v>
       </c>
       <c r="G29" t="n">
-        <v>0.01026032967390825</v>
+        <v>0.0103</v>
       </c>
       <c r="H29" t="n">
-        <v>0.06332597753187813</v>
+        <v>0.0633</v>
       </c>
       <c r="I29" t="n">
-        <v>0.1399637247335608</v>
+        <v>0.14</v>
       </c>
       <c r="J29" t="n">
         <v>0</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0001459459409588737</v>
-      </c>
-      <c r="L29" t="n">
-        <v>0.03973966602085729</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="30">
@@ -1692,25 +1603,22 @@
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.000437837822876621</v>
+        <v>0.0004</v>
       </c>
       <c r="G30" t="n">
-        <v>0.01026032967390825</v>
+        <v>0.0103</v>
       </c>
       <c r="H30" t="n">
-        <v>0.06332597753187813</v>
+        <v>0.0633</v>
       </c>
       <c r="I30" t="n">
-        <v>0.1399637247335608</v>
+        <v>0.14</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>0.0001459459409588737</v>
-      </c>
-      <c r="L30" t="n">
-        <v>0.03973966602085729</v>
+        <v>0.0179</v>
       </c>
     </row>
     <row r="31">
@@ -1734,25 +1642,22 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.002714582549559873</v>
+        <v>0.0027</v>
       </c>
       <c r="G31" t="n">
-        <v>0.02934362912851627</v>
+        <v>0.0293</v>
       </c>
       <c r="H31" t="n">
-        <v>0.1260507446137382</v>
+        <v>0.1261</v>
       </c>
       <c r="I31" t="n">
-        <v>0.2600415792191452</v>
+        <v>0.26</v>
       </c>
       <c r="J31" t="n">
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>0.000904860849853291</v>
-      </c>
-      <c r="L31" t="n">
-        <v>0.08235765176115038</v>
+        <v>0.0381</v>
       </c>
     </row>
     <row r="32">
@@ -1779,22 +1684,19 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>3.235015014246093e-05</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>0.00205884992735966</v>
+        <v>0.0021</v>
       </c>
       <c r="I32" t="n">
-        <v>0.01138180480603655</v>
+        <v>0.0114</v>
       </c>
       <c r="J32" t="n">
         <v>0</v>
       </c>
       <c r="K32" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" t="n">
-        <v>0.001957656926433522</v>
+        <v>0.0009</v>
       </c>
     </row>
     <row r="33">
@@ -1821,22 +1723,19 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>3.235015014246093e-05</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>0.00205884992735966</v>
+        <v>0.0021</v>
       </c>
       <c r="I33" t="n">
-        <v>0.01138180480603655</v>
+        <v>0.0114</v>
       </c>
       <c r="J33" t="n">
         <v>0</v>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" t="n">
-        <v>0.001957656926433522</v>
+        <v>0.0009</v>
       </c>
     </row>
     <row r="34">
@@ -1857,28 +1756,25 @@
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>0.004263282354625415</v>
+        <v>0.0043</v>
       </c>
       <c r="F34" t="n">
-        <v>0.02186921004427342</v>
+        <v>0.0219</v>
       </c>
       <c r="G34" t="n">
-        <v>0.06327948663655629</v>
+        <v>0.0633</v>
       </c>
       <c r="H34" t="n">
-        <v>0.2107781561396918</v>
+        <v>0.2108</v>
       </c>
       <c r="I34" t="n">
-        <v>0.3768784341464964</v>
+        <v>0.3769</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="K34" t="n">
-        <v>0.01013192491784142</v>
-      </c>
-      <c r="L34" t="n">
-        <v>0.1393540224510827</v>
+        <v>0.0741</v>
       </c>
     </row>
     <row r="35">
@@ -1902,25 +1798,22 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0001681340776008133</v>
+        <v>0.0002</v>
       </c>
       <c r="G35" t="n">
-        <v>0.009277398210473457</v>
+        <v>0.009299999999999999</v>
       </c>
       <c r="H35" t="n">
-        <v>0.05674783467615626</v>
+        <v>0.0567</v>
       </c>
       <c r="I35" t="n">
-        <v>0.1035408050587893</v>
+        <v>0.1035</v>
       </c>
       <c r="J35" t="n">
         <v>0</v>
       </c>
       <c r="K35" t="n">
-        <v>5.604469253360444e-05</v>
-      </c>
-      <c r="L35" t="n">
-        <v>0.03292793318293364</v>
+        <v>0.0147</v>
       </c>
     </row>
     <row r="36">
@@ -1947,22 +1840,19 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0.0004247329741154878</v>
+        <v>0.0004</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0386073014986532</v>
+        <v>0.0386</v>
       </c>
       <c r="I36" t="n">
-        <v>0.07041193154812152</v>
+        <v>0.0704</v>
       </c>
       <c r="J36" t="n">
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
-      </c>
-      <c r="L36" t="n">
-        <v>0.01871877492700067</v>
+        <v>0.0083</v>
       </c>
     </row>
     <row r="37">
@@ -1980,31 +1870,28 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>2.491562421045714e-05</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>0.01647931439678806</v>
+        <v>0.0165</v>
       </c>
       <c r="F37" t="n">
-        <v>0.03398437233585025</v>
+        <v>0.034</v>
       </c>
       <c r="G37" t="n">
-        <v>0.05582176575723141</v>
+        <v>0.0558</v>
       </c>
       <c r="H37" t="n">
-        <v>0.09846365966035799</v>
+        <v>0.0985</v>
       </c>
       <c r="I37" t="n">
-        <v>0.1360753301288614</v>
+        <v>0.1361</v>
       </c>
       <c r="J37" t="n">
-        <v>1.294990863329373e-06</v>
+        <v>0.0003</v>
       </c>
       <c r="K37" t="n">
-        <v>0.02231433370980879</v>
-      </c>
-      <c r="L37" t="n">
-        <v>0.0765139347794668</v>
+        <v>0.0529</v>
       </c>
     </row>
     <row r="38">
@@ -2028,25 +1915,22 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.0001681340776008133</v>
+        <v>0.0002</v>
       </c>
       <c r="G38" t="n">
-        <v>0.009277398210473457</v>
+        <v>0.009299999999999999</v>
       </c>
       <c r="H38" t="n">
-        <v>0.05674783467615626</v>
+        <v>0.0567</v>
       </c>
       <c r="I38" t="n">
-        <v>0.1035408050587893</v>
+        <v>0.1035</v>
       </c>
       <c r="J38" t="n">
         <v>0</v>
       </c>
       <c r="K38" t="n">
-        <v>5.604469253360444e-05</v>
-      </c>
-      <c r="L38" t="n">
-        <v>0.03292793318293364</v>
+        <v>0.0147</v>
       </c>
     </row>
     <row r="39">
@@ -2061,34 +1945,31 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.005967361416133518</v>
+        <v>0.006</v>
       </c>
       <c r="D39" t="n">
-        <v>0.005738064</v>
+        <v>0.0057</v>
       </c>
       <c r="E39" t="n">
-        <v>0.005724648227377284</v>
+        <v>0.0057</v>
       </c>
       <c r="F39" t="n">
-        <v>0.01206192299239135</v>
+        <v>0.0121</v>
       </c>
       <c r="G39" t="n">
-        <v>0.0391602079226817</v>
+        <v>0.0392</v>
       </c>
       <c r="H39" t="n">
-        <v>0.1131724317986836</v>
+        <v>0.1132</v>
       </c>
       <c r="I39" t="n">
-        <v>0.1894140945386769</v>
+        <v>0.1894</v>
       </c>
       <c r="J39" t="n">
-        <v>0.0009185440141510935</v>
+        <v>0.001</v>
       </c>
       <c r="K39" t="n">
-        <v>0.007837073149048638</v>
-      </c>
-      <c r="L39" t="n">
-        <v>0.07644499971868156</v>
+        <v>0.0407</v>
       </c>
     </row>
     <row r="40">
@@ -2103,34 +1984,31 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.005967361416133518</v>
+        <v>0.006</v>
       </c>
       <c r="D40" t="n">
-        <v>0.005738064</v>
+        <v>0.0057</v>
       </c>
       <c r="E40" t="n">
-        <v>0.005724648227377284</v>
+        <v>0.0057</v>
       </c>
       <c r="F40" t="n">
-        <v>0.01206192299239135</v>
+        <v>0.0121</v>
       </c>
       <c r="G40" t="n">
-        <v>0.0391602079226817</v>
+        <v>0.0392</v>
       </c>
       <c r="H40" t="n">
-        <v>0.1131724317986836</v>
+        <v>0.1132</v>
       </c>
       <c r="I40" t="n">
-        <v>0.1894140945386769</v>
+        <v>0.1894</v>
       </c>
       <c r="J40" t="n">
-        <v>0.0009185440141510935</v>
+        <v>0.001</v>
       </c>
       <c r="K40" t="n">
-        <v>0.007837073149048638</v>
-      </c>
-      <c r="L40" t="n">
-        <v>0.07644499971868156</v>
+        <v>0.0407</v>
       </c>
     </row>
     <row r="41">
@@ -2145,34 +2023,31 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="D41" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="E41" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="F41" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="G41" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="H41" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="I41" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="J41" t="n">
-        <v>0.01248280876581191</v>
+        <v>0.0137</v>
       </c>
       <c r="K41" t="n">
-        <v>0.08005641355140704</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
     </row>
     <row r="42">
@@ -2187,34 +2062,31 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="D42" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="E42" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="F42" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="G42" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="H42" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="I42" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="J42" t="n">
-        <v>0.00322441840337239</v>
+        <v>0.0035</v>
       </c>
       <c r="K42" t="n">
-        <v>0.0206792700269616</v>
-      </c>
-      <c r="L42" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
     </row>
     <row r="43">
@@ -2255,9 +2127,6 @@
       <c r="K43" t="n">
         <v>0</v>
       </c>
-      <c r="L43" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2286,19 +2155,16 @@
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0004859681109710256</v>
+        <v>0.0005</v>
       </c>
       <c r="I44" t="n">
-        <v>0.003836988658867257</v>
+        <v>0.0038</v>
       </c>
       <c r="J44" t="n">
         <v>0</v>
       </c>
       <c r="K44" t="n">
-        <v>0</v>
-      </c>
-      <c r="L44" t="n">
-        <v>0.0006011156101011635</v>
+        <v>0.0003</v>
       </c>
     </row>
     <row r="45">
@@ -2313,34 +2179,31 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.004908469010818952</v>
+        <v>0.0049</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0063314105967885</v>
+        <v>0.0063</v>
       </c>
       <c r="E45" t="n">
-        <v>0.006025597685702602</v>
+        <v>0.006</v>
       </c>
       <c r="F45" t="n">
-        <v>0.005903776007314022</v>
+        <v>0.0059</v>
       </c>
       <c r="G45" t="n">
-        <v>0.006525479822517292</v>
+        <v>0.0065</v>
       </c>
       <c r="H45" t="n">
-        <v>0.01402650143490848</v>
+        <v>0.014</v>
       </c>
       <c r="I45" t="n">
-        <v>0.02829197401831185</v>
+        <v>0.0283</v>
       </c>
       <c r="J45" t="n">
-        <v>0.0008393112587539712</v>
+        <v>0.0009</v>
       </c>
       <c r="K45" t="n">
-        <v>0.005984990459573076</v>
-      </c>
-      <c r="L45" t="n">
-        <v>0.01112154700008941</v>
+        <v>0.008200000000000001</v>
       </c>
     </row>
     <row r="46">
@@ -2355,34 +2218,31 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.004908469010818952</v>
+        <v>0.0049</v>
       </c>
       <c r="D46" t="n">
-        <v>0.0063314105967885</v>
+        <v>0.0063</v>
       </c>
       <c r="E46" t="n">
-        <v>0.006025597685702602</v>
+        <v>0.006</v>
       </c>
       <c r="F46" t="n">
-        <v>0.005903776007314022</v>
+        <v>0.0059</v>
       </c>
       <c r="G46" t="n">
-        <v>0.006525479822517292</v>
+        <v>0.0065</v>
       </c>
       <c r="H46" t="n">
-        <v>0.01402650143490848</v>
+        <v>0.014</v>
       </c>
       <c r="I46" t="n">
-        <v>0.02829197401831185</v>
+        <v>0.0283</v>
       </c>
       <c r="J46" t="n">
-        <v>0.0008393112587539712</v>
+        <v>0.0009</v>
       </c>
       <c r="K46" t="n">
-        <v>0.005984990459573076</v>
-      </c>
-      <c r="L46" t="n">
-        <v>0.01112154700008941</v>
+        <v>0.008200000000000001</v>
       </c>
     </row>
     <row r="47">
@@ -2397,34 +2257,31 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.004908469010818952</v>
+        <v>0.0049</v>
       </c>
       <c r="D47" t="n">
-        <v>0.0063314105967885</v>
+        <v>0.0063</v>
       </c>
       <c r="E47" t="n">
-        <v>0.006025597685702602</v>
+        <v>0.006</v>
       </c>
       <c r="F47" t="n">
-        <v>0.005903776007314022</v>
+        <v>0.0059</v>
       </c>
       <c r="G47" t="n">
-        <v>0.006525479822517292</v>
+        <v>0.0065</v>
       </c>
       <c r="H47" t="n">
-        <v>0.01402650143490848</v>
+        <v>0.014</v>
       </c>
       <c r="I47" t="n">
-        <v>0.02829197401831185</v>
+        <v>0.0283</v>
       </c>
       <c r="J47" t="n">
-        <v>0.0008393112587539712</v>
+        <v>0.0009</v>
       </c>
       <c r="K47" t="n">
-        <v>0.005984990459573076</v>
-      </c>
-      <c r="L47" t="n">
-        <v>0.01112154700008941</v>
+        <v>0.008200000000000001</v>
       </c>
     </row>
     <row r="48">
@@ -2439,34 +2296,31 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.004908469010818952</v>
+        <v>0.0049</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0063314105967885</v>
+        <v>0.0063</v>
       </c>
       <c r="E48" t="n">
-        <v>0.006025597685702602</v>
+        <v>0.006</v>
       </c>
       <c r="F48" t="n">
-        <v>0.005903776007314022</v>
+        <v>0.0059</v>
       </c>
       <c r="G48" t="n">
-        <v>0.006525479822517292</v>
+        <v>0.0065</v>
       </c>
       <c r="H48" t="n">
-        <v>0.01402650143490848</v>
+        <v>0.014</v>
       </c>
       <c r="I48" t="n">
-        <v>0.02829197401831185</v>
+        <v>0.0283</v>
       </c>
       <c r="J48" t="n">
-        <v>0.0008393112587539712</v>
+        <v>0.0009</v>
       </c>
       <c r="K48" t="n">
-        <v>0.005984990459573076</v>
-      </c>
-      <c r="L48" t="n">
-        <v>0.01112154700008941</v>
+        <v>0.008200000000000001</v>
       </c>
     </row>
     <row r="49">
@@ -2493,22 +2347,19 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>3.564003776540425e-06</v>
+        <v>0</v>
       </c>
       <c r="H49" t="n">
-        <v>0.001633255069512844</v>
+        <v>0.0016</v>
       </c>
       <c r="I49" t="n">
-        <v>0.006637015063650953</v>
+        <v>0.0066</v>
       </c>
       <c r="J49" t="n">
         <v>0</v>
       </c>
       <c r="K49" t="n">
-        <v>0</v>
-      </c>
-      <c r="L49" t="n">
-        <v>0.001240168152694918</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="50">
@@ -2535,22 +2386,19 @@
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>3.564003776540425e-06</v>
+        <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>0.001633255069512844</v>
+        <v>0.0016</v>
       </c>
       <c r="I50" t="n">
-        <v>0.006637015063650953</v>
+        <v>0.0066</v>
       </c>
       <c r="J50" t="n">
         <v>0</v>
       </c>
       <c r="K50" t="n">
-        <v>0</v>
-      </c>
-      <c r="L50" t="n">
-        <v>0.001240168152694918</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="51">
@@ -2571,28 +2419,25 @@
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>0.001388527543680859</v>
+        <v>0.0014</v>
       </c>
       <c r="F51" t="n">
-        <v>0.006937750597461727</v>
+        <v>0.0069</v>
       </c>
       <c r="G51" t="n">
-        <v>0.01628598878707258</v>
+        <v>0.0163</v>
       </c>
       <c r="H51" t="n">
-        <v>0.03178168353642778</v>
+        <v>0.0318</v>
       </c>
       <c r="I51" t="n">
-        <v>0.04625189492708107</v>
+        <v>0.0463</v>
       </c>
       <c r="J51" t="n">
         <v>0</v>
       </c>
       <c r="K51" t="n">
-        <v>0.003238268561607815</v>
-      </c>
-      <c r="L51" t="n">
-        <v>0.02390565074191244</v>
+        <v>0.0145</v>
       </c>
     </row>
     <row r="52">
@@ -2619,22 +2464,19 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>3.564003776540425e-06</v>
+        <v>0</v>
       </c>
       <c r="H52" t="n">
-        <v>0.001633255069512844</v>
+        <v>0.0016</v>
       </c>
       <c r="I52" t="n">
-        <v>0.006637015063650953</v>
+        <v>0.0066</v>
       </c>
       <c r="J52" t="n">
         <v>0</v>
       </c>
       <c r="K52" t="n">
-        <v>0</v>
-      </c>
-      <c r="L52" t="n">
-        <v>0.001240168152694918</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="53">
@@ -2661,22 +2503,19 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>3.564003776540425e-06</v>
+        <v>0</v>
       </c>
       <c r="H53" t="n">
-        <v>0.001633255069512844</v>
+        <v>0.0016</v>
       </c>
       <c r="I53" t="n">
-        <v>0.006637015063650953</v>
+        <v>0.0066</v>
       </c>
       <c r="J53" t="n">
         <v>0</v>
       </c>
       <c r="K53" t="n">
-        <v>0</v>
-      </c>
-      <c r="L53" t="n">
-        <v>0.001240168152694918</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="54">
@@ -2703,22 +2542,19 @@
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>3.564003776540425e-06</v>
+        <v>0</v>
       </c>
       <c r="H54" t="n">
-        <v>0.001633255069512844</v>
+        <v>0.0016</v>
       </c>
       <c r="I54" t="n">
-        <v>0.006637015063650953</v>
+        <v>0.0066</v>
       </c>
       <c r="J54" t="n">
         <v>0</v>
       </c>
       <c r="K54" t="n">
-        <v>0</v>
-      </c>
-      <c r="L54" t="n">
-        <v>0.001240168152694918</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="55">
@@ -2748,19 +2584,16 @@
         <v>0</v>
       </c>
       <c r="H55" t="n">
-        <v>0.001248323054600867</v>
+        <v>0.0012</v>
       </c>
       <c r="I55" t="n">
-        <v>0.006321334016694378</v>
+        <v>0.0063</v>
       </c>
       <c r="J55" t="n">
         <v>0</v>
       </c>
       <c r="K55" t="n">
-        <v>0</v>
-      </c>
-      <c r="L55" t="n">
-        <v>0.001102247515737014</v>
+        <v>0.0005</v>
       </c>
     </row>
     <row r="56">
@@ -2793,16 +2626,13 @@
         <v>0</v>
       </c>
       <c r="I56" t="n">
-        <v>0.00990071681390187</v>
+        <v>0.009900000000000001</v>
       </c>
       <c r="J56" t="n">
         <v>0</v>
       </c>
       <c r="K56" t="n">
-        <v>0</v>
-      </c>
-      <c r="L56" t="n">
-        <v>0.001237589601737734</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="57">
@@ -2832,19 +2662,16 @@
         <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>0.0001673042990286048</v>
+        <v>0.0002</v>
       </c>
       <c r="I57" t="n">
-        <v>0.005610066322755006</v>
+        <v>0.0056</v>
       </c>
       <c r="J57" t="n">
         <v>0</v>
       </c>
       <c r="K57" t="n">
-        <v>0</v>
-      </c>
-      <c r="L57" t="n">
-        <v>0.000743084365101527</v>
+        <v>0.0003</v>
       </c>
     </row>
     <row r="58">
@@ -2865,28 +2692,25 @@
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>0.001388527543680859</v>
+        <v>0.0014</v>
       </c>
       <c r="F58" t="n">
-        <v>0.006937750597461727</v>
+        <v>0.0069</v>
       </c>
       <c r="G58" t="n">
-        <v>0.01628598878707258</v>
+        <v>0.0163</v>
       </c>
       <c r="H58" t="n">
-        <v>0.03178168353642778</v>
+        <v>0.0318</v>
       </c>
       <c r="I58" t="n">
-        <v>0.04625189492708107</v>
+        <v>0.0463</v>
       </c>
       <c r="J58" t="n">
         <v>0</v>
       </c>
       <c r="K58" t="n">
-        <v>0.003238268561607815</v>
-      </c>
-      <c r="L58" t="n">
-        <v>0.02390565074191244</v>
+        <v>0.0145</v>
       </c>
     </row>
     <row r="59">
@@ -2927,9 +2751,6 @@
       <c r="K59" t="n">
         <v>0</v>
       </c>
-      <c r="L59" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2969,9 +2790,6 @@
       <c r="K60" t="n">
         <v>0</v>
       </c>
-      <c r="L60" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3011,9 +2829,6 @@
       <c r="K61" t="n">
         <v>0</v>
       </c>
-      <c r="L61" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3053,9 +2868,6 @@
       <c r="K62" t="n">
         <v>0</v>
       </c>
-      <c r="L62" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3095,9 +2907,6 @@
       <c r="K63" t="n">
         <v>0</v>
       </c>
-      <c r="L63" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3126,19 +2935,16 @@
         <v>0</v>
       </c>
       <c r="H64" t="n">
-        <v>0.003678721668662103</v>
+        <v>0.0037</v>
       </c>
       <c r="I64" t="n">
-        <v>0.01446162458746772</v>
+        <v>0.0145</v>
       </c>
       <c r="J64" t="n">
         <v>0</v>
       </c>
       <c r="K64" t="n">
-        <v>0</v>
-      </c>
-      <c r="L64" t="n">
-        <v>0.002727383490598991</v>
+        <v>0.0012</v>
       </c>
     </row>
     <row r="65">
@@ -3162,25 +2968,22 @@
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>0.001145686386901421</v>
+        <v>0.0011</v>
       </c>
       <c r="G65" t="n">
-        <v>0.007874579841060375</v>
+        <v>0.007900000000000001</v>
       </c>
       <c r="H65" t="n">
-        <v>0.02737904000267265</v>
+        <v>0.0274</v>
       </c>
       <c r="I65" t="n">
-        <v>0.06878423501571608</v>
+        <v>0.0688</v>
       </c>
       <c r="J65" t="n">
         <v>0</v>
       </c>
       <c r="K65" t="n">
-        <v>0.0003818954623004737</v>
-      </c>
-      <c r="L65" t="n">
-        <v>0.02036440177829541</v>
+        <v>0.0097</v>
       </c>
     </row>
     <row r="66">
@@ -3210,19 +3013,16 @@
         <v>0</v>
       </c>
       <c r="H66" t="n">
-        <v>0.008859783898023586</v>
+        <v>0.0089</v>
       </c>
       <c r="I66" t="n">
-        <v>0.02618587958711547</v>
+        <v>0.0262</v>
       </c>
       <c r="J66" t="n">
         <v>0</v>
       </c>
       <c r="K66" t="n">
-        <v>0</v>
-      </c>
-      <c r="L66" t="n">
-        <v>0.00548818092289533</v>
+        <v>0.0024</v>
       </c>
     </row>
     <row r="67">
@@ -3263,9 +3063,6 @@
       <c r="K67" t="n">
         <v>0</v>
       </c>
-      <c r="L67" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3291,22 +3088,19 @@
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>3.564003776540425e-06</v>
+        <v>0</v>
       </c>
       <c r="H68" t="n">
-        <v>0.001633255069512844</v>
+        <v>0.0016</v>
       </c>
       <c r="I68" t="n">
-        <v>0.006637015063650953</v>
+        <v>0.0066</v>
       </c>
       <c r="J68" t="n">
         <v>0</v>
       </c>
       <c r="K68" t="n">
-        <v>0</v>
-      </c>
-      <c r="L68" t="n">
-        <v>0.001240168152694918</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="69">
@@ -3333,22 +3127,19 @@
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>3.564003776540425e-06</v>
+        <v>0</v>
       </c>
       <c r="H69" t="n">
-        <v>0.001633255069512844</v>
+        <v>0.0016</v>
       </c>
       <c r="I69" t="n">
-        <v>0.006637015063650953</v>
+        <v>0.0066</v>
       </c>
       <c r="J69" t="n">
         <v>0</v>
       </c>
       <c r="K69" t="n">
-        <v>0</v>
-      </c>
-      <c r="L69" t="n">
-        <v>0.001240168152694918</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="70">
@@ -3375,22 +3166,19 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>3.564003776540425e-06</v>
+        <v>0</v>
       </c>
       <c r="H70" t="n">
-        <v>0.001633255069512844</v>
+        <v>0.0016</v>
       </c>
       <c r="I70" t="n">
-        <v>0.006637015063650953</v>
+        <v>0.0066</v>
       </c>
       <c r="J70" t="n">
         <v>0</v>
       </c>
       <c r="K70" t="n">
-        <v>0</v>
-      </c>
-      <c r="L70" t="n">
-        <v>0.001240168152694918</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="71">
@@ -3417,22 +3205,19 @@
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>3.564003776540425e-06</v>
+        <v>0</v>
       </c>
       <c r="H71" t="n">
-        <v>0.001633255069512844</v>
+        <v>0.0016</v>
       </c>
       <c r="I71" t="n">
-        <v>0.006637015063650953</v>
+        <v>0.0066</v>
       </c>
       <c r="J71" t="n">
         <v>0</v>
       </c>
       <c r="K71" t="n">
-        <v>0</v>
-      </c>
-      <c r="L71" t="n">
-        <v>0.001240168152694918</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="72">
@@ -3473,9 +3258,6 @@
       <c r="K72" t="n">
         <v>0</v>
       </c>
-      <c r="L72" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3501,22 +3283,19 @@
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>3.564003776540425e-06</v>
+        <v>0</v>
       </c>
       <c r="H73" t="n">
-        <v>0.001633255069512844</v>
+        <v>0.0016</v>
       </c>
       <c r="I73" t="n">
-        <v>0.006637015063650953</v>
+        <v>0.0066</v>
       </c>
       <c r="J73" t="n">
         <v>0</v>
       </c>
       <c r="K73" t="n">
-        <v>0</v>
-      </c>
-      <c r="L73" t="n">
-        <v>0.001240168152694918</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="74">
@@ -3543,22 +3322,19 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>3.564003776540425e-06</v>
+        <v>0</v>
       </c>
       <c r="H74" t="n">
-        <v>0.001633255069512844</v>
+        <v>0.0016</v>
       </c>
       <c r="I74" t="n">
-        <v>0.006637015063650953</v>
+        <v>0.0066</v>
       </c>
       <c r="J74" t="n">
         <v>0</v>
       </c>
       <c r="K74" t="n">
-        <v>0</v>
-      </c>
-      <c r="L74" t="n">
-        <v>0.001240168152694918</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="75">
@@ -3585,22 +3361,19 @@
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>3.564003776540425e-06</v>
+        <v>0</v>
       </c>
       <c r="H75" t="n">
-        <v>0.001633255069512844</v>
+        <v>0.0016</v>
       </c>
       <c r="I75" t="n">
-        <v>0.006637015063650953</v>
+        <v>0.0066</v>
       </c>
       <c r="J75" t="n">
         <v>0</v>
       </c>
       <c r="K75" t="n">
-        <v>0</v>
-      </c>
-      <c r="L75" t="n">
-        <v>0.001240168152694918</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="76">
@@ -3641,9 +3414,6 @@
       <c r="K76" t="n">
         <v>0</v>
       </c>
-      <c r="L76" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3683,9 +3453,6 @@
       <c r="K77" t="n">
         <v>0</v>
       </c>
-      <c r="L77" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3714,19 +3481,16 @@
         <v>0</v>
       </c>
       <c r="H78" t="n">
-        <v>0.001248323054600867</v>
+        <v>0.0012</v>
       </c>
       <c r="I78" t="n">
-        <v>0.006321334016694378</v>
+        <v>0.0063</v>
       </c>
       <c r="J78" t="n">
         <v>0</v>
       </c>
       <c r="K78" t="n">
-        <v>0</v>
-      </c>
-      <c r="L78" t="n">
-        <v>0.001102247515737014</v>
+        <v>0.0005</v>
       </c>
     </row>
     <row r="79">
@@ -3756,19 +3520,16 @@
         <v>0</v>
       </c>
       <c r="H79" t="n">
-        <v>0.002042243964229977</v>
+        <v>0.002</v>
       </c>
       <c r="I79" t="n">
-        <v>0.009840492483676898</v>
+        <v>0.0098</v>
       </c>
       <c r="J79" t="n">
         <v>0</v>
       </c>
       <c r="K79" t="n">
-        <v>0</v>
-      </c>
-      <c r="L79" t="n">
-        <v>0.001740622551517107</v>
+        <v>0.0008</v>
       </c>
     </row>
     <row r="80">
@@ -3789,28 +3550,25 @@
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>0.001388527543680859</v>
+        <v>0.0014</v>
       </c>
       <c r="F80" t="n">
-        <v>0.006937750597461727</v>
+        <v>0.0069</v>
       </c>
       <c r="G80" t="n">
-        <v>0.01628598878707258</v>
+        <v>0.0163</v>
       </c>
       <c r="H80" t="n">
-        <v>0.03178168353642778</v>
+        <v>0.0318</v>
       </c>
       <c r="I80" t="n">
-        <v>0.04625189492708107</v>
+        <v>0.0463</v>
       </c>
       <c r="J80" t="n">
         <v>0</v>
       </c>
       <c r="K80" t="n">
-        <v>0.003238268561607815</v>
-      </c>
-      <c r="L80" t="n">
-        <v>0.02390565074191244</v>
+        <v>0.0145</v>
       </c>
     </row>
     <row r="81">
@@ -3840,19 +3598,16 @@
         <v>0</v>
       </c>
       <c r="H81" t="n">
-        <v>0.001248323054600867</v>
+        <v>0.0012</v>
       </c>
       <c r="I81" t="n">
-        <v>0.006321334016694378</v>
+        <v>0.0063</v>
       </c>
       <c r="J81" t="n">
         <v>0</v>
       </c>
       <c r="K81" t="n">
-        <v>0</v>
-      </c>
-      <c r="L81" t="n">
-        <v>0.001102247515737014</v>
+        <v>0.0005</v>
       </c>
     </row>
     <row r="82">
@@ -3867,34 +3622,31 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0.004272773375639344</v>
+        <v>0.0043</v>
       </c>
       <c r="D82" t="n">
-        <v>0.005746170815058985</v>
+        <v>0.0057</v>
       </c>
       <c r="E82" t="n">
-        <v>0.005716536605960112</v>
+        <v>0.0057</v>
       </c>
       <c r="F82" t="n">
-        <v>0.005737520056000595</v>
+        <v>0.0057</v>
       </c>
       <c r="G82" t="n">
-        <v>0.006441720917693201</v>
+        <v>0.0064</v>
       </c>
       <c r="H82" t="n">
-        <v>0.01355357617654129</v>
+        <v>0.0136</v>
       </c>
       <c r="I82" t="n">
-        <v>0.02692316711234118</v>
+        <v>0.0269</v>
       </c>
       <c r="J82" t="n">
-        <v>0.0007428127633231639</v>
+        <v>0.0008</v>
       </c>
       <c r="K82" t="n">
-        <v>0.00572353108930694</v>
-      </c>
-      <c r="L82" t="n">
-        <v>0.01077986550673622</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="83">
@@ -3909,34 +3661,31 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.004272773375639344</v>
+        <v>0.0043</v>
       </c>
       <c r="D83" t="n">
-        <v>0.005746170815058985</v>
+        <v>0.0057</v>
       </c>
       <c r="E83" t="n">
-        <v>0.005716536605960112</v>
+        <v>0.0057</v>
       </c>
       <c r="F83" t="n">
-        <v>0.005737520056000595</v>
+        <v>0.0057</v>
       </c>
       <c r="G83" t="n">
-        <v>0.006441720917693201</v>
+        <v>0.0064</v>
       </c>
       <c r="H83" t="n">
-        <v>0.01355357617654129</v>
+        <v>0.0136</v>
       </c>
       <c r="I83" t="n">
-        <v>0.02692316711234118</v>
+        <v>0.0269</v>
       </c>
       <c r="J83" t="n">
-        <v>0.0007428127633231639</v>
+        <v>0.0008</v>
       </c>
       <c r="K83" t="n">
-        <v>0.00572353108930694</v>
-      </c>
-      <c r="L83" t="n">
-        <v>0.01077986550673622</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="84">
@@ -3966,19 +3715,16 @@
         <v>0</v>
       </c>
       <c r="H84" t="n">
-        <v>0.002624050609058154</v>
+        <v>0.0026</v>
       </c>
       <c r="I84" t="n">
-        <v>0.009085019476122605</v>
+        <v>0.0091</v>
       </c>
       <c r="J84" t="n">
         <v>0</v>
       </c>
       <c r="K84" t="n">
-        <v>0</v>
-      </c>
-      <c r="L84" t="n">
-        <v>0.001791640086779864</v>
+        <v>0.0008</v>
       </c>
     </row>
     <row r="85">
@@ -4008,19 +3754,16 @@
         <v>0</v>
       </c>
       <c r="H85" t="n">
-        <v>0.005084644734054182</v>
+        <v>0.0051</v>
       </c>
       <c r="I85" t="n">
-        <v>0.02116933243339376</v>
+        <v>0.0212</v>
       </c>
       <c r="J85" t="n">
         <v>0</v>
       </c>
       <c r="K85" t="n">
-        <v>0</v>
-      </c>
-      <c r="L85" t="n">
-        <v>0.003917327737687766</v>
+        <v>0.0017</v>
       </c>
     </row>
     <row r="86">
@@ -4050,19 +3793,16 @@
         <v>0</v>
       </c>
       <c r="H86" t="n">
-        <v>0.005995231149140136</v>
+        <v>0.006</v>
       </c>
       <c r="I86" t="n">
-        <v>0.01369946217492283</v>
+        <v>0.0137</v>
       </c>
       <c r="J86" t="n">
         <v>0</v>
       </c>
       <c r="K86" t="n">
-        <v>0</v>
-      </c>
-      <c r="L86" t="n">
-        <v>0.003211240559150388</v>
+        <v>0.0014</v>
       </c>
     </row>
     <row r="87">
@@ -4077,34 +3817,31 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="D87" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="E87" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="F87" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="G87" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="H87" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="I87" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
       <c r="J87" t="n">
-        <v>0.01248280876581191</v>
+        <v>0.0137</v>
       </c>
       <c r="K87" t="n">
-        <v>0.08005641355140704</v>
-      </c>
-      <c r="L87" t="n">
-        <v>0.08005641355140702</v>
+        <v>0.0801</v>
       </c>
     </row>
     <row r="88">
@@ -4119,34 +3856,31 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="D88" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="E88" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="F88" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="G88" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="H88" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="I88" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="J88" t="n">
-        <v>0.002232162171273926</v>
+        <v>0.0025</v>
       </c>
       <c r="K88" t="n">
-        <v>0.01431560005843678</v>
-      </c>
-      <c r="L88" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
     </row>
     <row r="89">
@@ -4187,9 +3921,6 @@
       <c r="K89" t="n">
         <v>0</v>
       </c>
-      <c r="L89" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4229,9 +3960,6 @@
       <c r="K90" t="n">
         <v>0</v>
       </c>
-      <c r="L90" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4245,34 +3973,31 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.00311222613773815</v>
+        <v>0.0031</v>
       </c>
       <c r="D91" t="n">
-        <v>0.004080909884948248</v>
+        <v>0.0041</v>
       </c>
       <c r="E91" t="n">
-        <v>0.005564131730834289</v>
+        <v>0.0056</v>
       </c>
       <c r="F91" t="n">
-        <v>0.006190207981067342</v>
+        <v>0.0062</v>
       </c>
       <c r="G91" t="n">
-        <v>0.006201847351673184</v>
+        <v>0.0062</v>
       </c>
       <c r="H91" t="n">
-        <v>0.005949891189305215</v>
+        <v>0.0059</v>
       </c>
       <c r="I91" t="n">
-        <v>0.005890573209834549</v>
+        <v>0.0059</v>
       </c>
       <c r="J91" t="n">
-        <v>0.0005356217339097998</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="K91" t="n">
-        <v>0.005772823814245306</v>
-      </c>
-      <c r="L91" t="n">
-        <v>0.006099949043351363</v>
+        <v>0.0062</v>
       </c>
     </row>
     <row r="92">
@@ -4287,34 +4012,31 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.00311222613773815</v>
+        <v>0.0031</v>
       </c>
       <c r="D92" t="n">
-        <v>0.004080909884948248</v>
+        <v>0.0041</v>
       </c>
       <c r="E92" t="n">
-        <v>0.005564131730834289</v>
+        <v>0.0056</v>
       </c>
       <c r="F92" t="n">
-        <v>0.006190207981067342</v>
+        <v>0.0062</v>
       </c>
       <c r="G92" t="n">
-        <v>0.006201847351673184</v>
+        <v>0.0062</v>
       </c>
       <c r="H92" t="n">
-        <v>0.005949891189305215</v>
+        <v>0.0059</v>
       </c>
       <c r="I92" t="n">
-        <v>0.005890573209834549</v>
+        <v>0.0059</v>
       </c>
       <c r="J92" t="n">
-        <v>0.0005356217339097998</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="K92" t="n">
-        <v>0.005772823814245306</v>
-      </c>
-      <c r="L92" t="n">
-        <v>0.006099949043351363</v>
+        <v>0.0062</v>
       </c>
     </row>
     <row r="93">
@@ -4329,34 +4051,31 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0.00311222613773815</v>
+        <v>0.0031</v>
       </c>
       <c r="D93" t="n">
-        <v>0.004080909884948248</v>
+        <v>0.0041</v>
       </c>
       <c r="E93" t="n">
-        <v>0.005564131730834289</v>
+        <v>0.0056</v>
       </c>
       <c r="F93" t="n">
-        <v>0.006190207981067342</v>
+        <v>0.0062</v>
       </c>
       <c r="G93" t="n">
-        <v>0.006201847351673184</v>
+        <v>0.0062</v>
       </c>
       <c r="H93" t="n">
-        <v>0.005949891189305215</v>
+        <v>0.0059</v>
       </c>
       <c r="I93" t="n">
-        <v>0.005890573209834549</v>
+        <v>0.0059</v>
       </c>
       <c r="J93" t="n">
-        <v>0.0005356217339097998</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="K93" t="n">
-        <v>0.005772823814245306</v>
-      </c>
-      <c r="L93" t="n">
-        <v>0.006099949043351363</v>
+        <v>0.0062</v>
       </c>
     </row>
     <row r="94">
@@ -4371,34 +4090,31 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0.00311222613773815</v>
+        <v>0.0031</v>
       </c>
       <c r="D94" t="n">
-        <v>0.004080909884948248</v>
+        <v>0.0041</v>
       </c>
       <c r="E94" t="n">
-        <v>0.005564131730834289</v>
+        <v>0.0056</v>
       </c>
       <c r="F94" t="n">
-        <v>0.006190207981067342</v>
+        <v>0.0062</v>
       </c>
       <c r="G94" t="n">
-        <v>0.006201847351673184</v>
+        <v>0.0062</v>
       </c>
       <c r="H94" t="n">
-        <v>0.005949891189305215</v>
+        <v>0.0059</v>
       </c>
       <c r="I94" t="n">
-        <v>0.005890573209834549</v>
+        <v>0.0059</v>
       </c>
       <c r="J94" t="n">
-        <v>0.0005356217339097998</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="K94" t="n">
-        <v>0.005772823814245306</v>
-      </c>
-      <c r="L94" t="n">
-        <v>0.006099949043351363</v>
+        <v>0.0062</v>
       </c>
     </row>
     <row r="95">
@@ -4439,9 +4155,6 @@
       <c r="K95" t="n">
         <v>0</v>
       </c>
-      <c r="L95" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4481,9 +4194,6 @@
       <c r="K96" t="n">
         <v>0</v>
       </c>
-      <c r="L96" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4509,22 +4219,19 @@
         <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>0.0002678262339805819</v>
+        <v>0.0003</v>
       </c>
       <c r="H97" t="n">
-        <v>0.002951082668989518</v>
+        <v>0.003</v>
       </c>
       <c r="I97" t="n">
-        <v>0.008924723741843738</v>
+        <v>0.0089</v>
       </c>
       <c r="J97" t="n">
         <v>0</v>
       </c>
       <c r="K97" t="n">
-        <v>0</v>
-      </c>
-      <c r="L97" t="n">
-        <v>0.002020752531215711</v>
+        <v>0.0009</v>
       </c>
     </row>
     <row r="98">
@@ -4565,9 +4272,6 @@
       <c r="K98" t="n">
         <v>0</v>
       </c>
-      <c r="L98" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4607,9 +4311,6 @@
       <c r="K99" t="n">
         <v>0</v>
       </c>
-      <c r="L99" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4649,9 +4350,6 @@
       <c r="K100" t="n">
         <v>0</v>
       </c>
-      <c r="L100" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4691,9 +4389,6 @@
       <c r="K101" t="n">
         <v>0</v>
       </c>
-      <c r="L101" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4733,9 +4428,6 @@
       <c r="K102" t="n">
         <v>0</v>
       </c>
-      <c r="L102" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4775,9 +4467,6 @@
       <c r="K103" t="n">
         <v>0</v>
       </c>
-      <c r="L103" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4817,9 +4506,6 @@
       <c r="K104" t="n">
         <v>0</v>
       </c>
-      <c r="L104" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4845,22 +4531,19 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>0.0002678262339805819</v>
+        <v>0.0003</v>
       </c>
       <c r="H105" t="n">
-        <v>0.002951082668989518</v>
+        <v>0.003</v>
       </c>
       <c r="I105" t="n">
-        <v>0.008924723741843738</v>
+        <v>0.0089</v>
       </c>
       <c r="J105" t="n">
         <v>0</v>
       </c>
       <c r="K105" t="n">
-        <v>0</v>
-      </c>
-      <c r="L105" t="n">
-        <v>0.002020752531215711</v>
+        <v>0.0009</v>
       </c>
     </row>
     <row r="106">
@@ -4901,9 +4584,6 @@
       <c r="K106" t="n">
         <v>0</v>
       </c>
-      <c r="L106" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4943,9 +4623,6 @@
       <c r="K107" t="n">
         <v>0</v>
       </c>
-      <c r="L107" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4985,9 +4662,6 @@
       <c r="K108" t="n">
         <v>0</v>
       </c>
-      <c r="L108" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -5027,9 +4701,6 @@
       <c r="K109" t="n">
         <v>0</v>
       </c>
-      <c r="L109" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -5069,9 +4740,6 @@
       <c r="K110" t="n">
         <v>0</v>
       </c>
-      <c r="L110" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -5111,9 +4779,6 @@
       <c r="K111" t="n">
         <v>0</v>
       </c>
-      <c r="L111" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -5153,9 +4818,6 @@
       <c r="K112" t="n">
         <v>0</v>
       </c>
-      <c r="L112" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -5184,19 +4846,16 @@
         <v>0</v>
       </c>
       <c r="H113" t="n">
-        <v>6.253294114735078e-05</v>
+        <v>0.0001</v>
       </c>
       <c r="I113" t="n">
-        <v>0.0007123467369293891</v>
+        <v>0.0007</v>
       </c>
       <c r="J113" t="n">
         <v>0</v>
       </c>
       <c r="K113" t="n">
         <v>0</v>
-      </c>
-      <c r="L113" t="n">
-        <v>0.0001046765774030113</v>
       </c>
     </row>
     <row r="114">
@@ -5237,9 +4896,6 @@
       <c r="K114" t="n">
         <v>0</v>
       </c>
-      <c r="L114" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -5279,9 +4935,6 @@
       <c r="K115" t="n">
         <v>0</v>
       </c>
-      <c r="L115" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -5321,9 +4974,6 @@
       <c r="K116" t="n">
         <v>0</v>
       </c>
-      <c r="L116" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -5363,9 +5013,6 @@
       <c r="K117" t="n">
         <v>0</v>
       </c>
-      <c r="L117" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5405,9 +5052,6 @@
       <c r="K118" t="n">
         <v>0</v>
       </c>
-      <c r="L118" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -5447,9 +5091,6 @@
       <c r="K119" t="n">
         <v>0</v>
       </c>
-      <c r="L119" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -5489,9 +5130,6 @@
       <c r="K120" t="n">
         <v>0</v>
       </c>
-      <c r="L120" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -5531,9 +5169,6 @@
       <c r="K121" t="n">
         <v>0</v>
       </c>
-      <c r="L121" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5573,9 +5208,6 @@
       <c r="K122" t="n">
         <v>0</v>
       </c>
-      <c r="L122" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -5615,9 +5247,6 @@
       <c r="K123" t="n">
         <v>0</v>
       </c>
-      <c r="L123" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5657,9 +5286,6 @@
       <c r="K124" t="n">
         <v>0</v>
       </c>
-      <c r="L124" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5699,9 +5325,6 @@
       <c r="K125" t="n">
         <v>0</v>
       </c>
-      <c r="L125" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5741,9 +5364,6 @@
       <c r="K126" t="n">
         <v>0</v>
       </c>
-      <c r="L126" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5783,9 +5403,6 @@
       <c r="K127" t="n">
         <v>0</v>
       </c>
-      <c r="L127" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -5825,9 +5442,6 @@
       <c r="K128" t="n">
         <v>0</v>
       </c>
-      <c r="L128" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -5867,9 +5481,6 @@
       <c r="K129" t="n">
         <v>0</v>
       </c>
-      <c r="L129" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -5909,9 +5520,6 @@
       <c r="K130" t="n">
         <v>0</v>
       </c>
-      <c r="L130" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -5951,9 +5559,6 @@
       <c r="K131" t="n">
         <v>0</v>
       </c>
-      <c r="L131" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -5979,22 +5584,19 @@
         <v>0</v>
       </c>
       <c r="G132" t="n">
-        <v>0.0002678262339805819</v>
+        <v>0.0003</v>
       </c>
       <c r="H132" t="n">
-        <v>0.002951082668989518</v>
+        <v>0.003</v>
       </c>
       <c r="I132" t="n">
-        <v>0.008924723741843738</v>
+        <v>0.0089</v>
       </c>
       <c r="J132" t="n">
         <v>0</v>
       </c>
       <c r="K132" t="n">
-        <v>0</v>
-      </c>
-      <c r="L132" t="n">
-        <v>0.002020752531215711</v>
+        <v>0.0009</v>
       </c>
     </row>
     <row r="133">
@@ -6035,9 +5637,6 @@
       <c r="K133" t="n">
         <v>0</v>
       </c>
-      <c r="L133" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -6051,34 +5650,31 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>0.002290039045430212</v>
+        <v>0.0023</v>
       </c>
       <c r="D134" t="n">
-        <v>0.003127343640359271</v>
+        <v>0.0031</v>
       </c>
       <c r="E134" t="n">
-        <v>0.004583034276696701</v>
+        <v>0.0046</v>
       </c>
       <c r="F134" t="n">
-        <v>0.005180538091091824</v>
+        <v>0.0052</v>
       </c>
       <c r="G134" t="n">
-        <v>0.005891767822413113</v>
+        <v>0.0059</v>
       </c>
       <c r="H134" t="n">
-        <v>0.005725964370748053</v>
+        <v>0.0057</v>
       </c>
       <c r="I134" t="n">
-        <v>0.005632975250334698</v>
+        <v>0.0056</v>
       </c>
       <c r="J134" t="n">
-        <v>0.0004005936450737887</v>
+        <v>0.0005</v>
       </c>
       <c r="K134" t="n">
-        <v>0.004782202214828409</v>
-      </c>
-      <c r="L134" t="n">
-        <v>0.005817967887987046</v>
+        <v>0.0055</v>
       </c>
     </row>
     <row r="135">
@@ -6093,34 +5689,31 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>0.002689564818213075</v>
+        <v>0.0027</v>
       </c>
       <c r="D135" t="n">
-        <v>0.003531534744100987</v>
+        <v>0.0035</v>
       </c>
       <c r="E135" t="n">
-        <v>0.004936255852220716</v>
+        <v>0.0049</v>
       </c>
       <c r="F135" t="n">
-        <v>0.005647997349038616</v>
+        <v>0.0056</v>
       </c>
       <c r="G135" t="n">
-        <v>0.005779409703167162</v>
+        <v>0.0058</v>
       </c>
       <c r="H135" t="n">
-        <v>0.005689183145128377</v>
+        <v>0.0057</v>
       </c>
       <c r="I135" t="n">
-        <v>0.005740317535994121</v>
+        <v>0.0057</v>
       </c>
       <c r="J135" t="n">
-        <v>0.0004631322443101423</v>
+        <v>0.0005</v>
       </c>
       <c r="K135" t="n">
-        <v>0.005173503017826682</v>
-      </c>
-      <c r="L135" t="n">
-        <v>0.005751966542760835</v>
+        <v>0.0057</v>
       </c>
     </row>
     <row r="136">
@@ -6135,34 +5728,31 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>0.001710844623739951</v>
+        <v>0.0017</v>
       </c>
       <c r="D136" t="n">
-        <v>0.002559017593983909</v>
+        <v>0.0026</v>
       </c>
       <c r="E136" t="n">
-        <v>0.003675416204390488</v>
+        <v>0.0037</v>
       </c>
       <c r="F136" t="n">
-        <v>0.004240864851219793</v>
+        <v>0.0042</v>
       </c>
       <c r="G136" t="n">
-        <v>0.006374757989668385</v>
+        <v>0.0064</v>
       </c>
       <c r="H136" t="n">
-        <v>0.005738064</v>
+        <v>0.0057</v>
       </c>
       <c r="I136" t="n">
-        <v>0.005738064</v>
+        <v>0.0057</v>
       </c>
       <c r="J136" t="n">
-        <v>0.0003108475489326305</v>
+        <v>0.0004</v>
       </c>
       <c r="K136" t="n">
-        <v>0.003863899086666923</v>
-      </c>
-      <c r="L136" t="n">
-        <v>0.006135997743542741</v>
+        <v>0.0051</v>
       </c>
     </row>
     <row r="137">
@@ -6177,34 +5767,31 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>0.002689564818213075</v>
+        <v>0.0027</v>
       </c>
       <c r="D137" t="n">
-        <v>0.003531534744100987</v>
+        <v>0.0035</v>
       </c>
       <c r="E137" t="n">
-        <v>0.004936255852220716</v>
+        <v>0.0049</v>
       </c>
       <c r="F137" t="n">
-        <v>0.005647997349038616</v>
+        <v>0.0056</v>
       </c>
       <c r="G137" t="n">
-        <v>0.005779409703167162</v>
+        <v>0.0058</v>
       </c>
       <c r="H137" t="n">
-        <v>0.005689183145128377</v>
+        <v>0.0057</v>
       </c>
       <c r="I137" t="n">
-        <v>0.005740317535994121</v>
+        <v>0.0057</v>
       </c>
       <c r="J137" t="n">
-        <v>0.0004631322443101423</v>
+        <v>0.0005</v>
       </c>
       <c r="K137" t="n">
-        <v>0.005173503017826682</v>
-      </c>
-      <c r="L137" t="n">
-        <v>0.005751966542760835</v>
+        <v>0.0057</v>
       </c>
     </row>
     <row r="138">
@@ -6245,9 +5832,6 @@
       <c r="K138" t="n">
         <v>0</v>
       </c>
-      <c r="L138" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -6261,34 +5845,31 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="D139" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="E139" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="F139" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="G139" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="H139" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="I139" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
       <c r="J139" t="n">
-        <v>0.00322441840337239</v>
+        <v>0.0035</v>
       </c>
       <c r="K139" t="n">
-        <v>0.0206792700269616</v>
-      </c>
-      <c r="L139" t="n">
-        <v>0.0206792700269616</v>
+        <v>0.0207</v>
       </c>
     </row>
     <row r="140">
@@ -6303,34 +5884,31 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="D140" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="E140" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="F140" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="G140" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="H140" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="I140" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
       <c r="J140" t="n">
-        <v>0.002232162171273926</v>
+        <v>0.0025</v>
       </c>
       <c r="K140" t="n">
-        <v>0.01431560005843678</v>
-      </c>
-      <c r="L140" t="n">
-        <v>0.01431560005843678</v>
+        <v>0.0143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>